<commit_message>
javascript level chart added
</commit_message>
<xml_diff>
--- a/pokeapp.xlsx
+++ b/pokeapp.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Oliver Thejl Eriksen\Documents\GitHub\PokeApp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{020742DC-9680-49F6-9679-DF14FB654401}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71C01E5A-8F5E-4E4B-81D2-32A75F792509}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-80" yWindow="-80" windowWidth="25760" windowHeight="13960" xr2:uid="{53F35512-1066-4FF8-91BC-6D4A4B044C9E}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" xr2:uid="{53F35512-1066-4FF8-91BC-6D4A4B044C9E}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark3" sheetId="3" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1519" uniqueCount="1518">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1534" uniqueCount="1533">
   <si>
     <t>Bulbasaur</t>
   </si>
@@ -4586,6 +4586,51 @@
   </si>
   <si>
     <t>Meloetta (Pirouette)</t>
+  </si>
+  <si>
+    <t>0.79530001</t>
+  </si>
+  <si>
+    <t>0.8003</t>
+  </si>
+  <si>
+    <t>0.8053</t>
+  </si>
+  <si>
+    <t>0.81029999</t>
+  </si>
+  <si>
+    <t>0.81529999</t>
+  </si>
+  <si>
+    <t>0.7928039467</t>
+  </si>
+  <si>
+    <t>0.797803922</t>
+  </si>
+  <si>
+    <t>0.8004150083</t>
+  </si>
+  <si>
+    <t>0.8054298091</t>
+  </si>
+  <si>
+    <t>0.8128038347</t>
+  </si>
+  <si>
+    <t>40.5</t>
+  </si>
+  <si>
+    <t>41.5</t>
+  </si>
+  <si>
+    <t>42.5</t>
+  </si>
+  <si>
+    <t>43.5</t>
+  </si>
+  <si>
+    <t>44.5</t>
   </si>
 </sst>
 </file>
@@ -4957,19 +5002,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A553CE7F-704B-4741-A6D2-C9C6BD65F3DC}">
-  <dimension ref="A1:B80"/>
+  <dimension ref="A1:C90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B80"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="7.26953125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.90625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>1341</v>
       </c>
@@ -4977,639 +5023,1076 @@
         <v>1342</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>1344</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C2" t="str">
+        <f>"["&amp;"'"&amp;A2&amp;"'"&amp;","&amp;"'"&amp;B2&amp;"'"&amp;"],"</f>
+        <v>['1','0.094'],</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>1343</v>
       </c>
       <c r="B3" t="s">
         <v>1345</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C3" t="str">
+        <f t="shared" ref="C3:C66" si="0">"["&amp;"'"&amp;A3&amp;"'"&amp;","&amp;"'"&amp;B3&amp;"'"&amp;"],"</f>
+        <v>['1.5','0.1351374318'],</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>2</v>
       </c>
       <c r="B4" t="s">
         <v>1346</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C4" t="str">
+        <f t="shared" si="0"/>
+        <v>['2','0.16639787'],</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>1347</v>
       </c>
       <c r="B5" t="s">
         <v>1348</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C5" t="str">
+        <f t="shared" si="0"/>
+        <v>['2.5','0.192650919'],</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>3</v>
       </c>
       <c r="B6" t="s">
         <v>1349</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C6" t="str">
+        <f t="shared" si="0"/>
+        <v>['3','0.21573247'],</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>1350</v>
       </c>
       <c r="B7" t="s">
         <v>1351</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C7" t="str">
+        <f t="shared" si="0"/>
+        <v>['3.5','0.2365726613'],</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>4</v>
       </c>
       <c r="B8" t="s">
         <v>1352</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C8" t="str">
+        <f t="shared" si="0"/>
+        <v>['4','0.25572005'],</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>1353</v>
       </c>
       <c r="B9" t="s">
         <v>1354</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C9" t="str">
+        <f t="shared" si="0"/>
+        <v>['4.5','0.2735303812'],</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>5</v>
       </c>
       <c r="B10" t="s">
         <v>1355</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C10" t="str">
+        <f t="shared" si="0"/>
+        <v>['5','0.29024988'],</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>1356</v>
       </c>
       <c r="B11" t="s">
         <v>1357</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C11" t="str">
+        <f t="shared" si="0"/>
+        <v>['5.5','0.3060573775'],</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>6</v>
       </c>
       <c r="B12" t="s">
         <v>1358</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C12" t="str">
+        <f t="shared" si="0"/>
+        <v>['6','0.3210876'],</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>1359</v>
       </c>
       <c r="B13" t="s">
         <v>1360</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C13" t="str">
+        <f t="shared" si="0"/>
+        <v>['6.5','0.3354450362'],</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>7</v>
       </c>
       <c r="B14" t="s">
         <v>1361</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C14" t="str">
+        <f t="shared" si="0"/>
+        <v>['7','0.34921268'],</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>1362</v>
       </c>
       <c r="B15" t="s">
         <v>1363</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C15" t="str">
+        <f t="shared" si="0"/>
+        <v>['7.5','0.3624577511'],</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>8</v>
       </c>
       <c r="B16" t="s">
         <v>1364</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C16" t="str">
+        <f t="shared" si="0"/>
+        <v>['8','0.3752356'],</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>1365</v>
       </c>
       <c r="B17" t="s">
         <v>1366</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C17" t="str">
+        <f t="shared" si="0"/>
+        <v>['8.5','0.387592416'],</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>9</v>
       </c>
       <c r="B18" t="s">
         <v>1367</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C18" t="str">
+        <f t="shared" si="0"/>
+        <v>['9','0.39956728'],</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>1368</v>
       </c>
       <c r="B19" t="s">
         <v>1369</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C19" t="str">
+        <f t="shared" si="0"/>
+        <v>['9.5','0.4111935514'],</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>10</v>
       </c>
       <c r="B20" t="s">
         <v>1370</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C20" t="str">
+        <f t="shared" si="0"/>
+        <v>['10','0.4225'],</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>1371</v>
       </c>
       <c r="B21" t="s">
         <v>1372</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C21" t="str">
+        <f t="shared" si="0"/>
+        <v>['10.5','0.4329264091'],</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>11</v>
       </c>
       <c r="B22" t="s">
         <v>1373</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C22" t="str">
+        <f t="shared" si="0"/>
+        <v>['11','0.44310755'],</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>1374</v>
       </c>
       <c r="B23" t="s">
         <v>1375</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C23" t="str">
+        <f t="shared" si="0"/>
+        <v>['11.5','0.4530599591'],</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>12</v>
       </c>
       <c r="B24" t="s">
         <v>1376</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C24" t="str">
+        <f t="shared" si="0"/>
+        <v>['12','0.4627984'],</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>1377</v>
       </c>
       <c r="B25" t="s">
         <v>1378</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C25" t="str">
+        <f t="shared" si="0"/>
+        <v>['12.5','0.472336093'],</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>13</v>
       </c>
       <c r="B26" t="s">
         <v>1379</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C26" t="str">
+        <f t="shared" si="0"/>
+        <v>['13','0.48168495'],</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>1380</v>
       </c>
       <c r="B27" t="s">
         <v>1381</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C27" t="str">
+        <f t="shared" si="0"/>
+        <v>['13.5','0.4908558003'],</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>14</v>
       </c>
       <c r="B28" t="s">
         <v>1382</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C28" t="str">
+        <f t="shared" si="0"/>
+        <v>['14','0.49985844'],</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>1383</v>
       </c>
       <c r="B29" t="s">
         <v>1384</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C29" t="str">
+        <f t="shared" si="0"/>
+        <v>['14.5','0.508701765'],</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>15</v>
       </c>
       <c r="B30" t="s">
         <v>1385</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C30" t="str">
+        <f t="shared" si="0"/>
+        <v>['15','0.51739395'],</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>1386</v>
       </c>
       <c r="B31" t="s">
         <v>1387</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C31" t="str">
+        <f t="shared" si="0"/>
+        <v>['15.5','0.5259425113'],</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>16</v>
       </c>
       <c r="B32" t="s">
         <v>1388</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C32" t="str">
+        <f t="shared" si="0"/>
+        <v>['16','0.5343543'],</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>1389</v>
       </c>
       <c r="B33" t="s">
         <v>1390</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C33" t="str">
+        <f t="shared" si="0"/>
+        <v>['16.5','0.5426357375'],</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>17</v>
       </c>
       <c r="B34" t="s">
         <v>1391</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C34" t="str">
+        <f t="shared" si="0"/>
+        <v>['17','0.5507927'],</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>1392</v>
       </c>
       <c r="B35" t="s">
         <v>1393</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C35" t="str">
+        <f t="shared" si="0"/>
+        <v>['17.5','0.5588305862'],</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>18</v>
       </c>
       <c r="B36" t="s">
         <v>1394</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C36" t="str">
+        <f t="shared" si="0"/>
+        <v>['18','0.5667545'],</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>1395</v>
       </c>
       <c r="B37" t="s">
         <v>1396</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C37" t="str">
+        <f t="shared" si="0"/>
+        <v>['18.5','0.5745691333'],</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>19</v>
       </c>
       <c r="B38" t="s">
         <v>1397</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C38" t="str">
+        <f t="shared" si="0"/>
+        <v>['19','0.5822789'],</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>1398</v>
       </c>
       <c r="B39" t="s">
         <v>1399</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C39" t="str">
+        <f t="shared" si="0"/>
+        <v>['19.5','0.5898879072'],</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>20</v>
       </c>
       <c r="B40" t="s">
         <v>1400</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C40" t="str">
+        <f t="shared" si="0"/>
+        <v>['20','0.5974'],</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>1401</v>
       </c>
       <c r="B41" t="s">
         <v>1402</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C41" t="str">
+        <f t="shared" si="0"/>
+        <v>['20.5','0.6048236651'],</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>21</v>
       </c>
       <c r="B42" t="s">
         <v>1403</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C42" t="str">
+        <f t="shared" si="0"/>
+        <v>['21','0.6121573'],</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>1404</v>
       </c>
       <c r="B43" t="s">
         <v>1405</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C43" t="str">
+        <f t="shared" si="0"/>
+        <v>['21.5','0.6194041216'],</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>22</v>
       </c>
       <c r="B44" t="s">
         <v>1406</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C44" t="str">
+        <f t="shared" si="0"/>
+        <v>['22','0.6265671'],</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>1407</v>
       </c>
       <c r="B45" t="s">
         <v>1408</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C45" t="str">
+        <f t="shared" si="0"/>
+        <v>['22.5','0.6336491432'],</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>23</v>
       </c>
       <c r="B46" t="s">
         <v>1409</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C46" t="str">
+        <f t="shared" si="0"/>
+        <v>['23','0.64065295'],</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>1410</v>
       </c>
       <c r="B47" t="s">
         <v>1411</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C47" t="str">
+        <f t="shared" si="0"/>
+        <v>['23.5','0.6475809666'],</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>24</v>
       </c>
       <c r="B48" t="s">
         <v>1412</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C48" t="str">
+        <f t="shared" si="0"/>
+        <v>['24','0.65443563'],</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>1413</v>
       </c>
       <c r="B49" t="s">
         <v>1414</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C49" t="str">
+        <f t="shared" si="0"/>
+        <v>['24.5','0.6612192524'],</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>25</v>
       </c>
       <c r="B50" t="s">
         <v>1415</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C50" t="str">
+        <f t="shared" si="0"/>
+        <v>['25','0.667934'],</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>1416</v>
       </c>
       <c r="B51" t="s">
         <v>1417</v>
       </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C51" t="str">
+        <f t="shared" si="0"/>
+        <v>['25.5','0.6745818959'],</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>26</v>
       </c>
       <c r="B52" t="s">
         <v>1418</v>
       </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C52" t="str">
+        <f t="shared" si="0"/>
+        <v>['26','0.6811649'],</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>1419</v>
       </c>
       <c r="B53" t="s">
         <v>1420</v>
       </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C53" t="str">
+        <f t="shared" si="0"/>
+        <v>['26.5','0.6876849038'],</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A54">
         <v>27</v>
       </c>
       <c r="B54" t="s">
         <v>1421</v>
       </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C54" t="str">
+        <f t="shared" si="0"/>
+        <v>['27','0.69414365'],</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>1422</v>
       </c>
       <c r="B55" t="s">
         <v>1423</v>
       </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C55" t="str">
+        <f t="shared" si="0"/>
+        <v>['27.5','0.70054287'],</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A56">
         <v>28</v>
       </c>
       <c r="B56" t="s">
         <v>1424</v>
       </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C56" t="str">
+        <f t="shared" si="0"/>
+        <v>['28','0.7068842'],</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>1425</v>
       </c>
       <c r="B57" t="s">
         <v>1426</v>
       </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C57" t="str">
+        <f t="shared" si="0"/>
+        <v>['28.5','0.7131691091'],</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A58">
         <v>29</v>
       </c>
       <c r="B58" t="s">
         <v>1427</v>
       </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C58" t="str">
+        <f t="shared" si="0"/>
+        <v>['29','0.7193991'],</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>1428</v>
       </c>
       <c r="B59" t="s">
         <v>1429</v>
       </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C59" t="str">
+        <f t="shared" si="0"/>
+        <v>['29.5','0.7255756136'],</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A60">
         <v>30</v>
       </c>
       <c r="B60" t="s">
         <v>1430</v>
       </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C60" t="str">
+        <f t="shared" si="0"/>
+        <v>['30','0.7317'],</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>1431</v>
       </c>
       <c r="B61" t="s">
         <v>1432</v>
       </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C61" t="str">
+        <f t="shared" si="0"/>
+        <v>['30.5','0.7347410093'],</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A62">
         <v>31</v>
       </c>
       <c r="B62" t="s">
         <v>1433</v>
       </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C62" t="str">
+        <f t="shared" si="0"/>
+        <v>['31','0.7377695'],</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>1434</v>
       </c>
       <c r="B63" t="s">
         <v>1435</v>
       </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C63" t="str">
+        <f t="shared" si="0"/>
+        <v>['31.5','0.7407855938'],</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A64">
         <v>32</v>
       </c>
       <c r="B64" t="s">
         <v>1436</v>
       </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C64" t="str">
+        <f t="shared" si="0"/>
+        <v>['32','0.74378943'],</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>1437</v>
       </c>
       <c r="B65" t="s">
         <v>1438</v>
       </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C65" t="str">
+        <f t="shared" si="0"/>
+        <v>['32.5','0.7467812109'],</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A66">
         <v>33</v>
       </c>
       <c r="B66" t="s">
         <v>1439</v>
       </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C66" t="str">
+        <f t="shared" si="0"/>
+        <v>['33','0.74976104'],</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>1440</v>
       </c>
       <c r="B67" t="s">
         <v>1441</v>
       </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C67" t="str">
+        <f t="shared" ref="C67:C90" si="1">"["&amp;"'"&amp;A67&amp;"'"&amp;","&amp;"'"&amp;B67&amp;"'"&amp;"],"</f>
+        <v>['33.5','0.7527290867'],</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A68">
         <v>34</v>
       </c>
       <c r="B68" t="s">
         <v>1442</v>
       </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C68" t="str">
+        <f t="shared" si="1"/>
+        <v>['34','0.7556855'],</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>1443</v>
       </c>
       <c r="B69" t="s">
         <v>1444</v>
       </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C69" t="str">
+        <f t="shared" si="1"/>
+        <v>['34.5','0.7586303683'],</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A70">
         <v>35</v>
       </c>
       <c r="B70" t="s">
         <v>1445</v>
       </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C70" t="str">
+        <f t="shared" si="1"/>
+        <v>['35','0.76156384'],</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>1446</v>
       </c>
       <c r="B71" t="s">
         <v>1447</v>
       </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C71" t="str">
+        <f t="shared" si="1"/>
+        <v>['35.5','0.7644860647'],</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A72">
         <v>36</v>
       </c>
       <c r="B72" t="s">
         <v>1448</v>
       </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C72" t="str">
+        <f t="shared" si="1"/>
+        <v>['36','0.76739717'],</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>1449</v>
       </c>
       <c r="B73" t="s">
         <v>1450</v>
       </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C73" t="str">
+        <f t="shared" si="1"/>
+        <v>['36.5','0.7702972656'],</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A74">
         <v>37</v>
       </c>
       <c r="B74" t="s">
         <v>1451</v>
       </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C74" t="str">
+        <f t="shared" si="1"/>
+        <v>['37','0.7731865'],</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>1452</v>
       </c>
       <c r="B75" t="s">
         <v>1453</v>
       </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C75" t="str">
+        <f t="shared" si="1"/>
+        <v>['37.5','0.7760649616'],</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A76">
         <v>38</v>
       </c>
       <c r="B76" t="s">
         <v>1454</v>
       </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C76" t="str">
+        <f t="shared" si="1"/>
+        <v>['38','0.77893275'],</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>1455</v>
       </c>
       <c r="B77" t="s">
         <v>1456</v>
       </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C77" t="str">
+        <f t="shared" si="1"/>
+        <v>['38.5','0.7817900548'],</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A78">
         <v>39</v>
       </c>
       <c r="B78" t="s">
         <v>1457</v>
       </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C78" t="str">
+        <f t="shared" si="1"/>
+        <v>['39','0.784637'],</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>1458</v>
       </c>
       <c r="B79" t="s">
         <v>1459</v>
       </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C79" t="str">
+        <f t="shared" si="1"/>
+        <v>['39.5','0.7874736075'],</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A80">
         <v>40</v>
       </c>
       <c r="B80" t="s">
         <v>1460</v>
       </c>
+      <c r="C80" t="str">
+        <f t="shared" si="1"/>
+        <v>['40','0.7903'],</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A81" t="s">
+        <v>1528</v>
+      </c>
+      <c r="B81" t="s">
+        <v>1523</v>
+      </c>
+      <c r="C81" t="str">
+        <f t="shared" si="1"/>
+        <v>['40.5','0.7928039467'],</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A82">
+        <v>41</v>
+      </c>
+      <c r="B82" t="s">
+        <v>1518</v>
+      </c>
+      <c r="C82" t="str">
+        <f t="shared" si="1"/>
+        <v>['41','0.79530001'],</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A83" t="s">
+        <v>1529</v>
+      </c>
+      <c r="B83" t="s">
+        <v>1524</v>
+      </c>
+      <c r="C83" t="str">
+        <f t="shared" si="1"/>
+        <v>['41.5','0.797803922'],</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A84">
+        <v>42</v>
+      </c>
+      <c r="B84" t="s">
+        <v>1519</v>
+      </c>
+      <c r="C84" t="str">
+        <f t="shared" si="1"/>
+        <v>['42','0.8003'],</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A85" t="s">
+        <v>1530</v>
+      </c>
+      <c r="B85" t="s">
+        <v>1525</v>
+      </c>
+      <c r="C85" t="str">
+        <f t="shared" si="1"/>
+        <v>['42.5','0.8004150083'],</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A86">
+        <v>43</v>
+      </c>
+      <c r="B86" t="s">
+        <v>1520</v>
+      </c>
+      <c r="C86" t="str">
+        <f t="shared" si="1"/>
+        <v>['43','0.8053'],</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A87" t="s">
+        <v>1531</v>
+      </c>
+      <c r="B87" t="s">
+        <v>1526</v>
+      </c>
+      <c r="C87" t="str">
+        <f t="shared" si="1"/>
+        <v>['43.5','0.8054298091'],</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A88">
+        <v>44</v>
+      </c>
+      <c r="B88" t="s">
+        <v>1521</v>
+      </c>
+      <c r="C88" t="str">
+        <f t="shared" si="1"/>
+        <v>['44','0.81029999'],</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A89" t="s">
+        <v>1532</v>
+      </c>
+      <c r="B89" t="s">
+        <v>1527</v>
+      </c>
+      <c r="C89" t="str">
+        <f t="shared" si="1"/>
+        <v>['44.5','0.8128038347'],</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A90">
+        <v>45</v>
+      </c>
+      <c r="B90" t="s">
+        <v>1522</v>
+      </c>
+      <c r="C90" t="str">
+        <f t="shared" si="1"/>
+        <v>['45','0.81529999'],</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>